<commit_message>
Added log of admixture iteration runs.
</commit_message>
<xml_diff>
--- a/admix log.xlsx
+++ b/admix log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elroy/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elroy/Documents/University/Honours 2019/Everything/BIOINFOMATICS/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,8 +26,22 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Ln_Prob</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -57,8 +71,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,152 +351,424 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15.6640625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>2</v>
-      </c>
-      <c r="C1">
-        <v>-300472584.39320999</v>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
+      <c r="C2" s="1">
+        <v>-300472584.39320999</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="C3" s="1">
+        <v>-300472457.15684301</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="C4" s="1">
+        <v>-300472452.21204299</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
+      <c r="C5" s="1">
+        <v>-300472661.58326</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>-296232690.30000001</v>
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-300472661.58326602</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-300472539.10000002</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-300472614.89999998</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-300472521.06</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-300472521.06</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>-292342966.60000002</v>
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-300472542.69999999</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-296232690.30000001</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-296203633.89999998</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-296203633.89999998</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-296232660.89999998</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>-288705996.89999998</v>
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-296232641.5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-296926334.05000001</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <f>-296310754.1</f>
+        <v>-296310754.10000002</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C19" s="1">
+        <v>-296206292.86000001</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>-296206304.04000002</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>6</v>
-      </c>
-      <c r="C21">
-        <v>-285228275.5</v>
+        <v>3</v>
+      </c>
+      <c r="C21" s="1">
+        <v>-296206718.19999999</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C22" s="1">
+        <v>-292342966.60000002</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>-292055931.23671103</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C24" s="1">
+        <v>-292704113.94526702</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>-292704113.94526702</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
+        <v>-292273276.63093001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>-292060816.89999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1">
+        <v>-292060816.89999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1">
+        <v>-292060816.89999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1">
+        <v>-292689450.80000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1">
+        <v>-292689607.30000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1">
+        <v>-288705996.89999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1">
+        <v>-288439777.38720101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="C34" s="1">
+        <v>-288922400.89754599</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1">
+        <v>-288922400.89754599</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="C36" s="1">
+        <v>-288487401.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="C37" s="1">
+        <v>-288922400.80000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="C38" s="1">
+        <v>-288922400.88999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="C39" s="1">
+        <v>-288487401.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1">
+        <v>-288487401.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="C41" s="1">
+        <v>-288406818.06</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="C42" s="1">
+        <v>-285228275.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>6</v>
+      </c>
+      <c r="C43" s="1">
+        <v>-285125760.20888197</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>6</v>
+      </c>
+      <c r="C44" s="1">
+        <v>-285296878.96076202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>6</v>
+      </c>
+      <c r="C45" s="1">
+        <v>-285296878.96076202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>6</v>
+      </c>
+      <c r="C46" s="1">
+        <v>-285125760.19999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>6</v>
+      </c>
+      <c r="C47" s="1">
+        <v>-285296878.95999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>6</v>
+      </c>
+      <c r="C48" s="1">
+        <v>-285180088.45999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>6</v>
+      </c>
+      <c r="C49" s="1">
+        <v>-285092038.80000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>6</v>
+      </c>
+      <c r="C50" s="1">
+        <v>-298509573.19999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>6</v>
+      </c>
+      <c r="C51" s="1">
+        <v>-285057013.60000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>